<commit_message>
next set of commits monday
</commit_message>
<xml_diff>
--- a/thesis_bibilo.xlsx
+++ b/thesis_bibilo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <r>
       <t>O'Rawe, J., Jiang, T., Sun, G., Wu, Y., Wang, W., Hu, J., ... &amp; Wei, Z. (2013). Low concordance of multiple variant-calling pipelines: practical implications for exome and genome sequencing. </t>
@@ -420,6 +420,284 @@
       </rPr>
       <t>, 113-141.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Rehm, H. L. (2017). Evolving health care through personal genomics. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature Reviews Genetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Angrist, M. (2016). Personal genomics: Where are we now?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied &amp; translational genomics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Escalona, M., Rocha, S., &amp; Posada, D. (2016). A comparison of tools for the simulation of genomic next-generation sequencing data. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature Reviews Genetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(8), 459-469.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Schirmer, M., D’Amore, R., Ijaz, U. Z., Hall, N., &amp; Quince, C. (2016). Illumina error profiles: resolving fine-scale variation in metagenomic sequencing data. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BMC bioinformatics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 125.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LeCun, Y., Bengio, Y., &amp; Hinton, G. (2015). Deep learning. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>521</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7553), 436-444.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kingma, D., &amp; Ba, J. (2014). Adam: A method for stochastic optimization. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:1412.6980</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sutskever, I., Martens, J., Dahl, G. E., &amp; Hinton, G. E. (2013). On the importance of initialization and momentum in deep learning. ICML (3), 28, 1139-1147.</t>
+  </si>
+  <si>
+    <r>
+      <t>Maas, A. L., Hannun, A. Y., &amp; Ng, A. Y. (2013, June). Rectifier nonlinearities improve neural network acoustic models. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proc. ICML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Vol. 30, No. 1).</t>
+    </r>
+  </si>
+  <si>
+    <t>Srivastava, N., Hinton, G. E., Krizhevsky, A., Sutskever, I., &amp; Salakhutdinov, R. (2014). Dropout: a simple way to prevent neural networks from overfitting. Journal of Machine Learning Research, 15(1), 1929-1958.</t>
+  </si>
+  <si>
+    <r>
+      <t>Ruder, S. (2016). An overview of gradient descent optimization algorithms. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:1609.04747</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Tieleman, T. and Hinton, G. Lecture 6.5 - RMSProp, COURSERA: Neural Networks for Machine Learning.
+Technical report, 2012</t>
   </si>
 </sst>
 </file>
@@ -786,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,6 +1216,61 @@
         <v>22</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>